<commit_message>
Opprydding, kjørte noen på ny for sikkerhets skyld
</commit_message>
<xml_diff>
--- a/kostraleveranse2020/Kostra 18 - Bruer under 10t.xlsx
+++ b/kostraleveranse2020/Kostra 18 - Bruer under 10t.xlsx
@@ -1,94 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DATA\leveranser\nvdbrapporter\lastned-nvdbrapporter\junk\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A4EB7A0-A64C-4C18-BCC7-9B9F3A0E88EE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="8550" yWindow="105" windowWidth="19275" windowHeight="15210" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
-    <sheet name="Bru aksellast under 10t" sheetId="1" r:id="rId1"/>
-    <sheet name="Metadata" sheetId="2" r:id="rId2"/>
+    <sheet name="Bru aksellast under 10t" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Metadata" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
-  <si>
-    <t>fylke</t>
-  </si>
-  <si>
-    <t>Antall</t>
-  </si>
-  <si>
-    <t>Lengde</t>
-  </si>
-  <si>
-    <t>Metadata</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t>Dato lagret</t>
-  </si>
-  <si>
-    <t>2021-02-04</t>
-  </si>
-  <si>
-    <t>egenskap</t>
-  </si>
-  <si>
-    <t>1263=7304</t>
-  </si>
-  <si>
-    <t>overlapp</t>
-  </si>
-  <si>
-    <t>904(10901=18186 OR 10901=18187 OR 10901=18188 OR 10901=18189 OR 10901=18190)</t>
-  </si>
-  <si>
-    <t>vegsystemreferanse</t>
-  </si>
-  <si>
-    <t>Fv</t>
-  </si>
-  <si>
-    <t>tidspunkt</t>
-  </si>
-  <si>
-    <t>2020-12-31</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <b val="1"/>
       <sz val="14"/>
-      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -104,27 +49,86 @@
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="overskrift" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
+    <cellStyle hidden="0" name="overskrift" xfId="1"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -412,212 +416,259 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="3" width="30" customWidth="1"/>
+    <col customWidth="1" max="1" min="1" width="30"/>
+    <col customWidth="1" max="2" min="2" width="30"/>
+    <col customWidth="1" max="3" min="3" width="30"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2">
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>fylke</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Antall</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Lengde</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
         <v>11</v>
       </c>
-      <c r="B2">
+      <c r="B2" t="n">
         <v>119</v>
       </c>
-      <c r="C2">
+      <c r="C2" t="n">
         <v>2855.612000000001</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3">
+    <row r="3">
+      <c r="A3" t="n">
         <v>15</v>
       </c>
-      <c r="B3">
+      <c r="B3" t="n">
         <v>142</v>
       </c>
-      <c r="C3">
-        <v>2774.5399999999991</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4">
+      <c r="C3" t="n">
+        <v>2774.539999999999</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
         <v>18</v>
       </c>
-      <c r="B4">
+      <c r="B4" t="n">
         <v>112</v>
       </c>
-      <c r="C4">
+      <c r="C4" t="n">
         <v>1983.691</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5">
+    <row r="5">
+      <c r="A5" t="n">
         <v>30</v>
       </c>
-      <c r="B5">
+      <c r="B5" t="n">
         <v>134</v>
       </c>
-      <c r="C5">
-        <v>4324.3149999999996</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6">
+      <c r="C5" t="n">
+        <v>4324.315</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
         <v>34</v>
       </c>
-      <c r="B6">
+      <c r="B6" t="n">
         <v>204</v>
       </c>
-      <c r="C6">
-        <v>4292.4200000000028</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7">
+      <c r="C6" t="n">
+        <v>4292.420000000003</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
         <v>38</v>
       </c>
-      <c r="B7">
+      <c r="B7" t="n">
         <v>33</v>
       </c>
-      <c r="C7">
-        <v>683.09999999999991</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8">
+      <c r="C7" t="n">
+        <v>683.0999999999999</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
         <v>42</v>
       </c>
-      <c r="B8">
+      <c r="B8" t="n">
         <v>140</v>
       </c>
-      <c r="C8">
+      <c r="C8" t="n">
         <v>2772.559999999999</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9">
+    <row r="9">
+      <c r="A9" t="n">
         <v>46</v>
       </c>
-      <c r="B9">
+      <c r="B9" t="n">
         <v>260</v>
       </c>
-      <c r="C9">
-        <v>3262.0029999999988</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10">
+      <c r="C9" t="n">
+        <v>3262.002999999999</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
         <v>50</v>
       </c>
-      <c r="B10">
+      <c r="B10" t="n">
         <v>186</v>
       </c>
-      <c r="C10">
+      <c r="C10" t="n">
         <v>4549.398000000001</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11">
+    <row r="11">
+      <c r="A11" t="n">
         <v>54</v>
       </c>
-      <c r="B11">
+      <c r="B11" t="n">
         <v>147</v>
       </c>
-      <c r="C11">
+      <c r="C11" t="n">
         <v>2132.33</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="2" width="30" customWidth="1"/>
+    <col customWidth="1" max="1" min="1" width="30"/>
+    <col customWidth="1" max="2" min="2" width="30"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" t="s">
-        <v>14</v>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Metadata</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Dato lagret</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>2021-02-04</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>egenskap</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>1263=7304</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>overlapp</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>904(10901=18186 OR 10901=18187 OR 10901=18188 OR 10901=18189 OR 10901=18190)</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>vegsystemreferanse</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Fv</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>tidspunkt</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>2020-12-31</t>
+        </is>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
</xml_diff>